<commit_message>
published state of ETDataset on 21th of June  201
</commit_message>
<xml_diff>
--- a/carriers_source_analyses/imported_electricity.carrier.xlsx
+++ b/carriers_source_analyses/imported_electricity.carrier.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31520" yWindow="-5320" windowWidth="41360" windowHeight="16280" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31520" yWindow="440" windowWidth="41360" windowHeight="16280" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -159,9 +159,6 @@
     <t>Date retrieved</t>
   </si>
   <si>
-    <t>Alexander Wirtz</t>
-  </si>
-  <si>
     <t>sustainable</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>Document</t>
-  </si>
-  <si>
-    <t>bio_ethanol</t>
   </si>
   <si>
     <t>%</t>
@@ -455,6 +449,12 @@
   <si>
     <t>Average cost per MJ electricity in Central West Europe</t>
   </si>
+  <si>
+    <t>imported_electricity</t>
+  </si>
+  <si>
+    <t>Mart Lubben</t>
+  </si>
 </sst>
 </file>
 
@@ -463,17 +463,24 @@
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="168" formatCode="0.00000"/>
-    <numFmt numFmtId="170" formatCode="0.0000000000"/>
-    <numFmt numFmtId="172" formatCode="0.00000000000000"/>
-    <numFmt numFmtId="174" formatCode="0.0000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.0000000000"/>
+    <numFmt numFmtId="168" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="33">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Lettertype hoofdtekst"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -992,654 +999,654 @@
   </borders>
   <cellStyleXfs count="362">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="21" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="22" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="183" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="9" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="10" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="24" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="170" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="172" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="fill"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="9" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="174" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="10" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="362">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2663,8 +2670,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2696,10 +2703,10 @@
     <row r="4" spans="1:4">
       <c r="A4" s="7"/>
       <c r="B4" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2708,7 +2715,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>36</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2856,7 +2863,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="B27" s="18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C27" s="130">
         <v>42227</v>
@@ -2864,17 +2871,17 @@
     </row>
     <row r="28" spans="1:4">
       <c r="C28" s="129" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="C29" s="129" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="C30" s="129" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -2891,7 +2898,7 @@
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -2916,30 +2923,30 @@
       <c r="G1" s="33"/>
     </row>
     <row r="2" spans="2:10" ht="15" customHeight="1">
-      <c r="B2" s="136" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="137"/>
-      <c r="D2" s="137"/>
-      <c r="E2" s="137"/>
-      <c r="F2" s="137"/>
-      <c r="G2" s="138"/>
+      <c r="B2" s="159" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="160"/>
+      <c r="D2" s="160"/>
+      <c r="E2" s="160"/>
+      <c r="F2" s="160"/>
+      <c r="G2" s="161"/>
     </row>
     <row r="3" spans="2:10">
-      <c r="B3" s="139"/>
-      <c r="C3" s="140"/>
-      <c r="D3" s="140"/>
-      <c r="E3" s="140"/>
-      <c r="F3" s="140"/>
-      <c r="G3" s="141"/>
+      <c r="B3" s="162"/>
+      <c r="C3" s="163"/>
+      <c r="D3" s="163"/>
+      <c r="E3" s="163"/>
+      <c r="F3" s="163"/>
+      <c r="G3" s="164"/>
     </row>
     <row r="4" spans="2:10" ht="63" customHeight="1">
-      <c r="B4" s="142"/>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="143"/>
-      <c r="F4" s="143"/>
-      <c r="G4" s="144"/>
+      <c r="B4" s="165"/>
+      <c r="C4" s="166"/>
+      <c r="D4" s="166"/>
+      <c r="E4" s="166"/>
+      <c r="F4" s="166"/>
+      <c r="G4" s="167"/>
     </row>
     <row r="5" spans="2:10" ht="17" thickBot="1">
       <c r="D5" s="33"/>
@@ -2990,7 +2997,7 @@
     <row r="9" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
       <c r="B9" s="23"/>
       <c r="C9" s="18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="18"/>
@@ -3003,7 +3010,7 @@
     <row r="10" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
       <c r="B10" s="23"/>
       <c r="C10" s="103" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>1</v>
@@ -3013,55 +3020,55 @@
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="110" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="30"/>
-      <c r="I10" s="145" t="s">
-        <v>94</v>
+      <c r="I10" s="136" t="s">
+        <v>92</v>
       </c>
       <c r="J10" s="42"/>
     </row>
     <row r="11" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
       <c r="B11" s="23"/>
       <c r="C11" s="110" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E11" s="133">
         <f>'Research data'!G7</f>
         <v>9.7222222222222224E-3</v>
       </c>
       <c r="F11" s="34"/>
-      <c r="G11" s="171" t="s">
-        <v>95</v>
+      <c r="G11" s="158" t="s">
+        <v>93</v>
       </c>
       <c r="H11" s="30"/>
-      <c r="I11" s="145" t="s">
-        <v>93</v>
+      <c r="I11" s="136" t="s">
+        <v>91</v>
       </c>
       <c r="J11" s="42"/>
     </row>
     <row r="12" spans="2:10" s="41" customFormat="1" ht="20" thickBot="1">
       <c r="B12" s="23"/>
       <c r="C12" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="166">
+        <v>41</v>
+      </c>
+      <c r="E12" s="153">
         <f>'Research data'!G8</f>
         <v>0.14645479910501019</v>
       </c>
       <c r="F12" s="34"/>
       <c r="G12" s="134" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H12" s="30"/>
-      <c r="I12" s="145" t="s">
-        <v>62</v>
+      <c r="I12" s="136" t="s">
+        <v>60</v>
       </c>
       <c r="J12" s="42"/>
     </row>
@@ -3193,7 +3200,7 @@
     <row r="5" spans="2:18" ht="17" thickBot="1">
       <c r="B5" s="74"/>
       <c r="C5" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="32"/>
       <c r="E5" s="32"/>
@@ -3218,10 +3225,10 @@
         <v>sustainable</v>
       </c>
       <c r="D6" s="112" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="112" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F6" s="22" t="s">
         <v>1</v>
@@ -3232,7 +3239,7 @@
       <c r="H6" s="77"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
-      <c r="K6" s="170"/>
+      <c r="K6" s="157"/>
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
@@ -3248,22 +3255,22 @@
         <v>cost_per_mj</v>
       </c>
       <c r="D7" s="113" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="113" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="169">
+        <v>44</v>
+      </c>
+      <c r="G7" s="156">
         <f>K7</f>
         <v>9.7222222222222224E-3</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="K7" s="169">
+      <c r="K7" s="156">
         <f>Notes!F48</f>
         <v>9.7222222222222224E-3</v>
       </c>
@@ -3282,15 +3289,15 @@
         <v>co2_conversion_per_mj</v>
       </c>
       <c r="D8" s="113" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="113" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="113" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="168">
+      <c r="G8" s="155">
         <f>I8</f>
         <v>0.14645479910501019</v>
       </c>
@@ -3470,7 +3477,7 @@
     <row r="7" spans="2:12">
       <c r="B7" s="49"/>
       <c r="C7" s="122" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="57"/>
       <c r="E7" s="119"/>
@@ -3485,11 +3492,11 @@
     <row r="8" spans="2:12">
       <c r="B8" s="49"/>
       <c r="C8" s="135" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D8" s="58"/>
       <c r="E8" s="120" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F8" s="120"/>
       <c r="G8" s="57" t="s">
@@ -3503,39 +3510,39 @@
       </c>
       <c r="J8" s="57"/>
       <c r="K8" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" s="61" t="s">
         <v>61</v>
-      </c>
-      <c r="L8" s="61" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="49"/>
       <c r="C9" s="57"/>
       <c r="D9" s="58"/>
-      <c r="E9" s="167" t="s">
-        <v>86</v>
+      <c r="E9" s="154" t="s">
+        <v>84</v>
       </c>
       <c r="F9" s="119"/>
       <c r="G9" s="52"/>
       <c r="H9" s="53" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J9" s="53"/>
       <c r="K9" s="53" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L9" s="67" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="49"/>
       <c r="C10" s="123" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="58"/>
       <c r="E10" s="119"/>
@@ -3602,7 +3609,7 @@
     <row r="15" spans="2:12">
       <c r="B15" s="49"/>
       <c r="C15" s="57" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" s="57"/>
       <c r="E15" s="57"/>
@@ -3678,7 +3685,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:BL558"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -3702,7 +3709,7 @@
         <v>25</v>
       </c>
       <c r="D2" s="108" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E2" s="108"/>
       <c r="F2" s="108" t="s">
@@ -3813,16 +3820,16 @@
       <c r="J6" s="114"/>
       <c r="K6" s="114"/>
       <c r="L6" s="114"/>
-      <c r="M6" s="146" t="s">
-        <v>65</v>
-      </c>
-      <c r="N6" s="147"/>
-      <c r="O6" s="147"/>
-      <c r="P6" s="147"/>
-      <c r="Q6" s="147"/>
-      <c r="R6" s="147"/>
-      <c r="S6" s="147"/>
-      <c r="T6" s="147"/>
+      <c r="M6" s="137" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="138"/>
+      <c r="O6" s="138"/>
+      <c r="P6" s="138"/>
+      <c r="Q6" s="138"/>
+      <c r="R6" s="138"/>
+      <c r="S6" s="138"/>
+      <c r="T6" s="138"/>
       <c r="V6" s="114"/>
       <c r="W6" s="114"/>
       <c r="X6" s="114"/>
@@ -3843,16 +3850,16 @@
       <c r="J7" s="114"/>
       <c r="K7" s="114"/>
       <c r="L7" s="114"/>
-      <c r="M7" s="148" t="s">
+      <c r="M7" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="148"/>
-      <c r="O7" s="148"/>
-      <c r="P7" s="148"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="148"/>
-      <c r="S7" s="148"/>
-      <c r="T7" s="148"/>
+      <c r="N7" s="170"/>
+      <c r="O7" s="170"/>
+      <c r="P7" s="170"/>
+      <c r="Q7" s="170"/>
+      <c r="R7" s="170"/>
+      <c r="S7" s="170"/>
+      <c r="T7" s="170"/>
       <c r="V7" s="114"/>
       <c r="W7" s="114"/>
       <c r="X7" s="114"/>
@@ -3872,18 +3879,18 @@
       <c r="J8" s="114"/>
       <c r="K8" s="114"/>
       <c r="L8" s="114"/>
-      <c r="M8" s="147"/>
-      <c r="N8" s="147" t="s">
-        <v>66</v>
-      </c>
-      <c r="O8" s="147"/>
-      <c r="P8" s="147"/>
-      <c r="Q8" s="147"/>
-      <c r="R8" s="147" t="s">
-        <v>67</v>
-      </c>
-      <c r="S8" s="147"/>
-      <c r="T8" s="147"/>
+      <c r="M8" s="138"/>
+      <c r="N8" s="138" t="s">
+        <v>64</v>
+      </c>
+      <c r="O8" s="138"/>
+      <c r="P8" s="138"/>
+      <c r="Q8" s="138"/>
+      <c r="R8" s="138" t="s">
+        <v>65</v>
+      </c>
+      <c r="S8" s="138"/>
+      <c r="T8" s="138"/>
       <c r="V8" s="114"/>
       <c r="W8" s="114"/>
       <c r="X8" s="114"/>
@@ -3902,18 +3909,18 @@
       <c r="J9" s="114"/>
       <c r="K9" s="114"/>
       <c r="L9" s="114"/>
-      <c r="M9" s="147"/>
-      <c r="N9" s="148" t="s">
+      <c r="M9" s="138"/>
+      <c r="N9" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="149"/>
-      <c r="R9" s="148" t="s">
+      <c r="O9" s="170"/>
+      <c r="P9" s="170"/>
+      <c r="Q9" s="171"/>
+      <c r="R9" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="S9" s="148"/>
-      <c r="T9" s="148"/>
+      <c r="S9" s="170"/>
+      <c r="T9" s="170"/>
       <c r="V9" s="114"/>
       <c r="W9" s="114"/>
       <c r="X9" s="114"/>
@@ -3929,14 +3936,14 @@
       <c r="J10" s="114"/>
       <c r="K10" s="114"/>
       <c r="L10" s="114"/>
-      <c r="M10" s="147"/>
-      <c r="N10" s="150"/>
-      <c r="O10" s="151"/>
-      <c r="P10" s="151"/>
-      <c r="Q10" s="151"/>
-      <c r="R10" s="150"/>
-      <c r="S10" s="151"/>
-      <c r="T10" s="151"/>
+      <c r="M10" s="138"/>
+      <c r="N10" s="139"/>
+      <c r="O10" s="140"/>
+      <c r="P10" s="140"/>
+      <c r="Q10" s="140"/>
+      <c r="R10" s="139"/>
+      <c r="S10" s="140"/>
+      <c r="T10" s="140"/>
       <c r="V10" s="114"/>
       <c r="W10" s="114"/>
       <c r="X10" s="114"/>
@@ -3946,39 +3953,39 @@
       <c r="B11" s="105"/>
       <c r="C11" s="114"/>
       <c r="D11" s="114"/>
-      <c r="F11" s="165">
+      <c r="F11" s="152">
         <f>N32</f>
         <v>0.52723727677803667</v>
       </c>
       <c r="G11" s="114" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H11" s="116"/>
       <c r="I11" s="114"/>
       <c r="J11" s="114"/>
       <c r="K11" s="114"/>
       <c r="L11" s="114"/>
-      <c r="M11" s="152"/>
-      <c r="N11" s="152" t="s">
+      <c r="M11" s="141"/>
+      <c r="N11" s="141" t="s">
+        <v>66</v>
+      </c>
+      <c r="O11" s="141" t="s">
+        <v>67</v>
+      </c>
+      <c r="P11" s="141" t="s">
         <v>68</v>
       </c>
-      <c r="O11" s="152" t="s">
+      <c r="Q11" s="141" t="s">
         <v>69</v>
       </c>
-      <c r="P11" s="152" t="s">
+      <c r="R11" s="141" t="s">
+        <v>66</v>
+      </c>
+      <c r="S11" s="141" t="s">
         <v>70</v>
       </c>
-      <c r="Q11" s="152" t="s">
+      <c r="T11" s="141" t="s">
         <v>71</v>
-      </c>
-      <c r="R11" s="152" t="s">
-        <v>68</v>
-      </c>
-      <c r="S11" s="152" t="s">
-        <v>72</v>
-      </c>
-      <c r="T11" s="152" t="s">
-        <v>73</v>
       </c>
       <c r="V11" s="114"/>
       <c r="W11" s="114"/>
@@ -3995,21 +4002,21 @@
         <v>527</v>
       </c>
       <c r="G12" s="114" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H12" s="114"/>
       <c r="I12" s="114"/>
       <c r="J12" s="114"/>
       <c r="K12" s="114"/>
       <c r="L12" s="114"/>
-      <c r="M12" s="147"/>
-      <c r="N12" s="147"/>
-      <c r="O12" s="147"/>
-      <c r="P12" s="147"/>
-      <c r="Q12" s="147"/>
-      <c r="R12" s="147"/>
-      <c r="S12" s="153"/>
-      <c r="T12" s="147"/>
+      <c r="M12" s="138"/>
+      <c r="N12" s="138"/>
+      <c r="O12" s="138"/>
+      <c r="P12" s="138"/>
+      <c r="Q12" s="138"/>
+      <c r="R12" s="138"/>
+      <c r="S12" s="142"/>
+      <c r="T12" s="138"/>
       <c r="V12" s="114"/>
       <c r="W12" s="114"/>
       <c r="X12" s="114"/>
@@ -4025,23 +4032,23 @@
         <v>3.6</v>
       </c>
       <c r="G13" s="114" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H13" s="114"/>
       <c r="I13" s="114"/>
       <c r="J13" s="114"/>
       <c r="K13" s="114"/>
       <c r="L13" s="114"/>
-      <c r="M13" s="148" t="s">
+      <c r="M13" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="N13" s="148"/>
-      <c r="O13" s="148"/>
-      <c r="P13" s="148"/>
-      <c r="Q13" s="148"/>
-      <c r="R13" s="148"/>
-      <c r="S13" s="148"/>
-      <c r="T13" s="148"/>
+      <c r="N13" s="170"/>
+      <c r="O13" s="170"/>
+      <c r="P13" s="170"/>
+      <c r="Q13" s="170"/>
+      <c r="R13" s="170"/>
+      <c r="S13" s="170"/>
+      <c r="T13" s="170"/>
       <c r="V13" s="114"/>
       <c r="W13" s="114"/>
       <c r="X13" s="114"/>
@@ -4057,21 +4064,21 @@
         <v>0.14645479910501019</v>
       </c>
       <c r="G14" s="114" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H14" s="114"/>
       <c r="I14" s="114"/>
       <c r="J14" s="114"/>
       <c r="K14" s="114"/>
       <c r="L14" s="114"/>
-      <c r="M14" s="150"/>
-      <c r="N14" s="151"/>
-      <c r="O14" s="151"/>
-      <c r="P14" s="151"/>
-      <c r="Q14" s="151"/>
-      <c r="R14" s="151"/>
-      <c r="S14" s="151"/>
-      <c r="T14" s="151"/>
+      <c r="M14" s="139"/>
+      <c r="N14" s="140"/>
+      <c r="O14" s="140"/>
+      <c r="P14" s="140"/>
+      <c r="Q14" s="140"/>
+      <c r="R14" s="140"/>
+      <c r="S14" s="140"/>
+      <c r="T14" s="140"/>
       <c r="V14" s="114"/>
       <c r="W14" s="114"/>
       <c r="X14" s="114"/>
@@ -4089,25 +4096,25 @@
       <c r="J15" s="114"/>
       <c r="K15" s="114"/>
       <c r="L15" s="114"/>
-      <c r="M15" s="150"/>
-      <c r="N15" s="154" t="s">
+      <c r="M15" s="139"/>
+      <c r="N15" s="143" t="s">
+        <v>72</v>
+      </c>
+      <c r="O15" s="143" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="143" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q15" s="143"/>
+      <c r="R15" s="143" t="s">
         <v>74</v>
       </c>
-      <c r="O15" s="154" t="s">
+      <c r="S15" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="P15" s="154" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q15" s="154"/>
-      <c r="R15" s="154" t="s">
-        <v>76</v>
-      </c>
-      <c r="S15" s="155" t="s">
-        <v>77</v>
-      </c>
-      <c r="T15" s="154" t="s">
-        <v>53</v>
+      <c r="T15" s="143" t="s">
+        <v>51</v>
       </c>
       <c r="V15" s="114"/>
       <c r="W15" s="114"/>
@@ -4126,14 +4133,14 @@
       <c r="J16" s="114"/>
       <c r="K16" s="114"/>
       <c r="L16" s="114"/>
-      <c r="M16" s="147"/>
-      <c r="N16" s="147"/>
-      <c r="O16" s="147"/>
-      <c r="P16" s="147"/>
-      <c r="Q16" s="147"/>
-      <c r="R16" s="147"/>
-      <c r="S16" s="153"/>
-      <c r="T16" s="147"/>
+      <c r="M16" s="138"/>
+      <c r="N16" s="138"/>
+      <c r="O16" s="138"/>
+      <c r="P16" s="138"/>
+      <c r="Q16" s="138"/>
+      <c r="R16" s="138"/>
+      <c r="S16" s="142"/>
+      <c r="T16" s="138"/>
       <c r="V16" s="114"/>
       <c r="W16" s="114"/>
       <c r="X16" s="114"/>
@@ -4150,28 +4157,28 @@
       <c r="J17" s="114"/>
       <c r="K17" s="114"/>
       <c r="L17" s="114"/>
-      <c r="M17" s="156">
+      <c r="M17" s="145">
         <v>2000</v>
       </c>
-      <c r="N17" s="162">
+      <c r="N17" s="149">
         <v>0.54527000939004366</v>
       </c>
-      <c r="O17" s="162">
+      <c r="O17" s="149">
         <v>8.2672486839821993</v>
       </c>
-      <c r="P17" s="162">
+      <c r="P17" s="149">
         <v>43.545321274476755</v>
       </c>
-      <c r="Q17" s="162">
+      <c r="Q17" s="149">
         <v>40.539801764085702</v>
       </c>
-      <c r="R17" s="163">
+      <c r="R17" s="150">
         <v>0.6411633901125442</v>
       </c>
-      <c r="S17" s="163">
+      <c r="S17" s="150">
         <v>8.9931269836050642</v>
       </c>
-      <c r="T17" s="163">
+      <c r="T17" s="150">
         <v>40.030570084943612</v>
       </c>
       <c r="V17" s="114"/>
@@ -4190,28 +4197,28 @@
       <c r="J18" s="114"/>
       <c r="K18" s="114"/>
       <c r="L18" s="114"/>
-      <c r="M18" s="156">
+      <c r="M18" s="145">
         <v>2001</v>
       </c>
-      <c r="N18" s="162">
+      <c r="N18" s="149">
         <v>0.55870272508963847</v>
       </c>
-      <c r="O18" s="162">
+      <c r="O18" s="149">
         <v>8.4551074906673769</v>
       </c>
-      <c r="P18" s="162">
+      <c r="P18" s="149">
         <v>42.577814699264636</v>
       </c>
-      <c r="Q18" s="162">
+      <c r="Q18" s="149">
         <v>39.61480428178583</v>
       </c>
-      <c r="R18" s="163">
+      <c r="R18" s="150">
         <v>0.64641878966078092</v>
       </c>
-      <c r="S18" s="163">
+      <c r="S18" s="150">
         <v>9.1359691554843394</v>
       </c>
-      <c r="T18" s="163">
+      <c r="T18" s="150">
         <v>39.404686451233403</v>
       </c>
       <c r="V18" s="114"/>
@@ -4230,28 +4237,28 @@
       <c r="J19" s="114"/>
       <c r="K19" s="114"/>
       <c r="L19" s="114"/>
-      <c r="M19" s="156">
+      <c r="M19" s="145">
         <v>2002</v>
       </c>
-      <c r="N19" s="162">
+      <c r="N19" s="149">
         <v>0.55483294760982504</v>
       </c>
-      <c r="O19" s="162">
+      <c r="O19" s="149">
         <v>8.3804496959004577</v>
       </c>
-      <c r="P19" s="162">
+      <c r="P19" s="149">
         <v>42.957121999802048</v>
       </c>
-      <c r="Q19" s="162">
+      <c r="Q19" s="149">
         <v>39.966946978373571</v>
       </c>
-      <c r="R19" s="163">
+      <c r="R19" s="150">
         <v>0.64576122793758828</v>
       </c>
-      <c r="S19" s="163">
+      <c r="S19" s="150">
         <v>9.1396089020600737</v>
       </c>
-      <c r="T19" s="163">
+      <c r="T19" s="150">
         <v>39.388993977505514</v>
       </c>
       <c r="V19" s="114"/>
@@ -4270,28 +4277,28 @@
       <c r="J20" s="114"/>
       <c r="K20" s="114"/>
       <c r="L20" s="114"/>
-      <c r="M20" s="156">
+      <c r="M20" s="145">
         <v>2003</v>
       </c>
-      <c r="N20" s="162">
+      <c r="N20" s="149">
         <v>0.55362915713024408</v>
       </c>
-      <c r="O20" s="162">
+      <c r="O20" s="149">
         <v>8.3772189677036391</v>
       </c>
-      <c r="P20" s="162">
+      <c r="P20" s="149">
         <v>42.973688689276692</v>
       </c>
-      <c r="Q20" s="162">
+      <c r="Q20" s="149">
         <v>39.970588725348186</v>
       </c>
-      <c r="R20" s="163">
+      <c r="R20" s="150">
         <v>0.63938251109596345</v>
       </c>
-      <c r="S20" s="163">
+      <c r="S20" s="150">
         <v>9.0909755241275381</v>
       </c>
-      <c r="T20" s="163">
+      <c r="T20" s="150">
         <v>39.599710619015141</v>
       </c>
       <c r="V20" s="114"/>
@@ -4310,28 +4317,28 @@
       <c r="J21" s="114"/>
       <c r="K21" s="114"/>
       <c r="L21" s="114"/>
-      <c r="M21" s="156">
+      <c r="M21" s="145">
         <v>2004</v>
       </c>
-      <c r="N21" s="162">
+      <c r="N21" s="149">
         <v>0.53437979858847884</v>
       </c>
-      <c r="O21" s="162">
+      <c r="O21" s="149">
         <v>8.1473364296802391</v>
       </c>
-      <c r="P21" s="162">
+      <c r="P21" s="149">
         <v>44.186220012781405</v>
       </c>
-      <c r="Q21" s="162">
+      <c r="Q21" s="149">
         <v>41.020895467565332</v>
       </c>
-      <c r="R21" s="163">
+      <c r="R21" s="150">
         <v>0.62377295431400848</v>
       </c>
-      <c r="S21" s="163">
+      <c r="S21" s="150">
         <v>8.9616215255162235</v>
       </c>
-      <c r="T21" s="163">
+      <c r="T21" s="150">
         <v>40.171301474290125</v>
       </c>
       <c r="V21" s="114"/>
@@ -4350,28 +4357,28 @@
       <c r="J22" s="114"/>
       <c r="K22" s="114"/>
       <c r="L22" s="114"/>
-      <c r="M22" s="156">
+      <c r="M22" s="145">
         <v>2005</v>
       </c>
-      <c r="N22" s="162">
+      <c r="N22" s="149">
         <v>0.51415325255652977</v>
       </c>
-      <c r="O22" s="162">
+      <c r="O22" s="149">
         <v>7.9067583743866052</v>
       </c>
-      <c r="P22" s="162">
+      <c r="P22" s="149">
         <v>45.530669201451133</v>
       </c>
-      <c r="Q22" s="162">
+      <c r="Q22" s="149">
         <v>42.272065855461868</v>
       </c>
-      <c r="R22" s="163">
+      <c r="R22" s="150">
         <v>0.61548550323403872</v>
       </c>
-      <c r="S22" s="163">
+      <c r="S22" s="150">
         <v>8.9315712789822115</v>
       </c>
-      <c r="T22" s="163">
+      <c r="T22" s="150">
         <v>40.306457705505032</v>
       </c>
       <c r="V22" s="114"/>
@@ -4390,28 +4397,28 @@
       <c r="J23" s="114"/>
       <c r="K23" s="114"/>
       <c r="L23" s="114"/>
-      <c r="M23" s="156">
+      <c r="M23" s="145">
         <v>2006</v>
       </c>
-      <c r="N23" s="162">
+      <c r="N23" s="149">
         <v>0.50359122654455701</v>
       </c>
-      <c r="O23" s="162">
+      <c r="O23" s="149">
         <v>7.6632657574358118</v>
       </c>
-      <c r="P23" s="162">
+      <c r="P23" s="149">
         <v>46.977360748671046</v>
       </c>
-      <c r="Q23" s="162">
+      <c r="Q23" s="149">
         <v>43.62415681780265</v>
       </c>
-      <c r="R23" s="163">
+      <c r="R23" s="150">
         <v>0.61099799160185031</v>
       </c>
-      <c r="S23" s="163">
+      <c r="S23" s="150">
         <v>8.7393847554257622</v>
       </c>
-      <c r="T23" s="163">
+      <c r="T23" s="150">
         <v>41.192831083045924</v>
       </c>
       <c r="V23" s="114"/>
@@ -4430,28 +4437,28 @@
       <c r="J24" s="114"/>
       <c r="K24" s="114"/>
       <c r="L24" s="114"/>
-      <c r="M24" s="156">
+      <c r="M24" s="145">
         <v>2007</v>
       </c>
-      <c r="N24" s="162">
+      <c r="N24" s="149">
         <v>0.50035039665156722</v>
       </c>
-      <c r="O24" s="162">
+      <c r="O24" s="149">
         <v>7.6842121517038366</v>
       </c>
-      <c r="P24" s="162">
+      <c r="P24" s="149">
         <v>46.849305158782798</v>
       </c>
-      <c r="Q24" s="162">
+      <c r="Q24" s="149">
         <v>43.494076651852318</v>
       </c>
-      <c r="R24" s="163">
+      <c r="R24" s="150">
         <v>0.59826025610283451</v>
       </c>
-      <c r="S24" s="163">
+      <c r="S24" s="150">
         <v>8.6764091990098979</v>
       </c>
-      <c r="T24" s="163">
+      <c r="T24" s="150">
         <v>41.491818993631739</v>
       </c>
       <c r="V24" s="114"/>
@@ -4470,28 +4477,28 @@
       <c r="J25" s="114"/>
       <c r="K25" s="114"/>
       <c r="L25" s="114"/>
-      <c r="M25" s="156">
+      <c r="M25" s="145">
         <v>2008</v>
       </c>
-      <c r="N25" s="162">
+      <c r="N25" s="149">
         <v>0.48873994886347027</v>
       </c>
-      <c r="O25" s="162">
+      <c r="O25" s="149">
         <v>7.5815898491011167</v>
       </c>
-      <c r="P25" s="162">
+      <c r="P25" s="149">
         <v>47.483444391638002</v>
       </c>
-      <c r="Q25" s="162">
+      <c r="Q25" s="149">
         <v>43.994864632173865</v>
       </c>
-      <c r="R25" s="163">
+      <c r="R25" s="150">
         <v>0.6076306997312636</v>
       </c>
-      <c r="S25" s="163">
+      <c r="S25" s="150">
         <v>8.8220196919222111</v>
       </c>
-      <c r="T25" s="163">
+      <c r="T25" s="150">
         <v>40.806982139206767</v>
       </c>
       <c r="V25" s="114"/>
@@ -4510,28 +4517,28 @@
       <c r="J26" s="114"/>
       <c r="K26" s="114"/>
       <c r="L26" s="114"/>
-      <c r="M26" s="156">
+      <c r="M26" s="145">
         <v>2009</v>
       </c>
-      <c r="N26" s="162">
+      <c r="N26" s="149">
         <v>0.47623912587215478</v>
       </c>
-      <c r="O26" s="162">
+      <c r="O26" s="149">
         <v>7.4147408804397559</v>
       </c>
-      <c r="P26" s="162">
+      <c r="P26" s="149">
         <v>48.551932670996997</v>
       </c>
-      <c r="Q26" s="162">
+      <c r="Q26" s="149">
         <v>44.958021669468629</v>
       </c>
-      <c r="R26" s="163">
+      <c r="R26" s="150">
         <v>0.59042284005562362</v>
       </c>
-      <c r="S26" s="163">
+      <c r="S26" s="150">
         <v>8.6491955296669847</v>
       </c>
-      <c r="T26" s="163">
+      <c r="T26" s="150">
         <v>41.622368087897861</v>
       </c>
       <c r="V26" s="114"/>
@@ -4550,28 +4557,28 @@
       <c r="J27" s="114"/>
       <c r="K27" s="114"/>
       <c r="L27" s="114"/>
-      <c r="M27" s="156">
+      <c r="M27" s="145">
         <v>2010</v>
       </c>
-      <c r="N27" s="162">
+      <c r="N27" s="149">
         <v>0.46036340459707753</v>
       </c>
-      <c r="O27" s="162">
+      <c r="O27" s="149">
         <v>7.2315657302176186</v>
       </c>
-      <c r="P27" s="162">
+      <c r="P27" s="149">
         <v>49.781750374709873</v>
       </c>
-      <c r="Q27" s="162">
+      <c r="Q27" s="149">
         <v>45.996176119924009</v>
       </c>
-      <c r="R27" s="163">
+      <c r="R27" s="150">
         <v>0.567996290027867</v>
       </c>
-      <c r="S27" s="163">
+      <c r="S27" s="150">
         <v>8.4262493025249885</v>
       </c>
-      <c r="T27" s="163">
+      <c r="T27" s="150">
         <v>42.72363504508742</v>
       </c>
       <c r="V27" s="114"/>
@@ -4583,28 +4590,28 @@
       <c r="B28" s="105"/>
       <c r="K28" s="114"/>
       <c r="L28" s="114"/>
-      <c r="M28" s="157">
+      <c r="M28" s="146">
         <v>2011</v>
       </c>
-      <c r="N28" s="162">
+      <c r="N28" s="149">
         <v>0.44210219761142849</v>
       </c>
-      <c r="O28" s="162">
+      <c r="O28" s="149">
         <v>6.96630937893406</v>
       </c>
-      <c r="P28" s="162">
+      <c r="P28" s="149">
         <v>51.677291434777608</v>
       </c>
-      <c r="Q28" s="162">
+      <c r="Q28" s="149">
         <v>47.821014152311008</v>
       </c>
-      <c r="R28" s="163">
+      <c r="R28" s="150">
         <v>0.55557901106191254</v>
       </c>
-      <c r="S28" s="163">
+      <c r="S28" s="150">
         <v>8.2481999152389154</v>
       </c>
-      <c r="T28" s="163">
+      <c r="T28" s="150">
         <v>43.645886823727935</v>
       </c>
       <c r="V28" s="114"/>
@@ -4615,142 +4622,142 @@
     <row r="29" spans="2:25" customFormat="1">
       <c r="B29" s="105"/>
       <c r="C29" s="114"/>
-      <c r="M29" s="146">
+      <c r="M29" s="137">
         <v>2012</v>
       </c>
-      <c r="N29" s="162">
+      <c r="N29" s="149">
         <v>0.47189640266606458</v>
       </c>
-      <c r="O29" s="162">
+      <c r="O29" s="149">
         <v>7.1436114287050323</v>
       </c>
-      <c r="P29" s="162">
+      <c r="P29" s="149">
         <v>50.394678321026696</v>
       </c>
-      <c r="Q29" s="162">
+      <c r="Q29" s="149">
         <v>46.92409565696088</v>
       </c>
-      <c r="R29" s="163">
+      <c r="R29" s="150">
         <v>0.60776111465098903</v>
       </c>
-      <c r="S29" s="163">
+      <c r="S29" s="150">
         <v>8.5455908294539373</v>
       </c>
-      <c r="T29" s="163">
+      <c r="T29" s="150">
         <v>42.126987727892889</v>
       </c>
     </row>
     <row r="30" spans="2:25" customFormat="1">
       <c r="B30" s="105"/>
       <c r="C30" s="114"/>
-      <c r="M30" s="146">
+      <c r="M30" s="137">
         <v>2013</v>
       </c>
-      <c r="N30" s="162">
+      <c r="N30" s="149">
         <v>0.48093326220982524</v>
       </c>
-      <c r="O30" s="162">
+      <c r="O30" s="149">
         <v>7.1001964810056872</v>
       </c>
-      <c r="P30" s="162">
+      <c r="P30" s="149">
         <v>50.702822233591029</v>
       </c>
-      <c r="Q30" s="162">
+      <c r="Q30" s="149">
         <v>47.194255971082448</v>
       </c>
-      <c r="R30" s="163">
+      <c r="R30" s="150">
         <v>0.62205757886678981</v>
       </c>
-      <c r="S30" s="163">
+      <c r="S30" s="150">
         <v>8.4503942980665698</v>
       </c>
-      <c r="T30" s="163">
+      <c r="T30" s="150">
         <v>42.601562400747042</v>
       </c>
     </row>
     <row r="31" spans="2:25" customFormat="1">
       <c r="B31" s="105"/>
       <c r="C31" s="114"/>
-      <c r="M31" s="146">
+      <c r="M31" s="137">
         <v>2014</v>
       </c>
-      <c r="N31" s="162">
+      <c r="N31" s="149">
         <v>0.50305777964528764</v>
       </c>
-      <c r="O31" s="162">
+      <c r="O31" s="149">
         <v>7.3631196341779415</v>
       </c>
-      <c r="P31" s="162">
+      <c r="P31" s="149">
         <v>48.892319816312799</v>
       </c>
-      <c r="Q31" s="162">
+      <c r="Q31" s="149">
         <v>45.740023751539056</v>
       </c>
-      <c r="R31" s="163">
+      <c r="R31" s="150">
         <v>0.63639721312929931</v>
       </c>
-      <c r="S31" s="163">
+      <c r="S31" s="150">
         <v>8.6504818158902452</v>
       </c>
-      <c r="T31" s="163">
+      <c r="T31" s="150">
         <v>41.61617903626</v>
       </c>
     </row>
     <row r="32" spans="2:25" customFormat="1" ht="21">
       <c r="B32" s="105"/>
       <c r="C32" s="114"/>
-      <c r="M32" s="158" t="s">
-        <v>78</v>
-      </c>
-      <c r="N32" s="164">
+      <c r="M32" s="147" t="s">
+        <v>76</v>
+      </c>
+      <c r="N32" s="151">
         <v>0.52723727677803667</v>
       </c>
-      <c r="O32" s="162">
+      <c r="O32" s="149">
         <v>7.3079224938204517</v>
       </c>
-      <c r="P32" s="162">
+      <c r="P32" s="149">
         <v>49.261606195798393</v>
       </c>
-      <c r="Q32" s="162">
+      <c r="Q32" s="149">
         <v>46.413521172361648</v>
       </c>
-      <c r="R32" s="163">
+      <c r="R32" s="150">
         <v>0.67765971611763232</v>
       </c>
-      <c r="S32" s="163">
+      <c r="S32" s="150">
         <v>8.6903398742149083</v>
       </c>
-      <c r="T32" s="163">
+      <c r="T32" s="150">
         <v>41.42530731947037</v>
       </c>
     </row>
     <row r="33" spans="2:20" customFormat="1">
       <c r="B33" s="105"/>
       <c r="C33" s="114"/>
-      <c r="M33" s="148" t="s">
+      <c r="M33" s="170" t="s">
         <v>1</v>
       </c>
-      <c r="N33" s="148"/>
-      <c r="O33" s="148"/>
-      <c r="P33" s="148"/>
-      <c r="Q33" s="148"/>
-      <c r="R33" s="148"/>
-      <c r="S33" s="148"/>
-      <c r="T33" s="148"/>
+      <c r="N33" s="170"/>
+      <c r="O33" s="170"/>
+      <c r="P33" s="170"/>
+      <c r="Q33" s="170"/>
+      <c r="R33" s="170"/>
+      <c r="S33" s="170"/>
+      <c r="T33" s="170"/>
     </row>
     <row r="34" spans="2:20" customFormat="1">
       <c r="B34" s="105"/>
       <c r="C34" s="114"/>
-      <c r="M34" s="147" t="s">
-        <v>79</v>
-      </c>
-      <c r="N34" s="159"/>
-      <c r="O34" s="159"/>
-      <c r="P34" s="159"/>
-      <c r="Q34" s="159"/>
-      <c r="R34" s="159"/>
-      <c r="S34" s="159"/>
-      <c r="T34" s="159"/>
+      <c r="M34" s="138" t="s">
+        <v>77</v>
+      </c>
+      <c r="N34" s="148"/>
+      <c r="O34" s="148"/>
+      <c r="P34" s="148"/>
+      <c r="Q34" s="148"/>
+      <c r="R34" s="148"/>
+      <c r="S34" s="148"/>
+      <c r="T34" s="148"/>
     </row>
     <row r="35" spans="2:20" customFormat="1">
       <c r="B35" s="105"/>
@@ -4759,48 +4766,48 @@
     <row r="36" spans="2:20" customFormat="1">
       <c r="B36" s="105"/>
       <c r="C36" s="114"/>
-      <c r="M36" s="160" t="s">
-        <v>80</v>
-      </c>
-      <c r="N36" s="160"/>
-      <c r="O36" s="160"/>
-      <c r="P36" s="160"/>
-      <c r="Q36" s="160"/>
-      <c r="R36" s="160"/>
-      <c r="S36" s="160"/>
+      <c r="M36" s="168" t="s">
+        <v>78</v>
+      </c>
+      <c r="N36" s="168"/>
+      <c r="O36" s="168"/>
+      <c r="P36" s="168"/>
+      <c r="Q36" s="168"/>
+      <c r="R36" s="168"/>
+      <c r="S36" s="168"/>
     </row>
     <row r="37" spans="2:20" customFormat="1">
       <c r="B37" s="105"/>
       <c r="C37" s="114"/>
-      <c r="M37" s="160" t="s">
-        <v>81</v>
-      </c>
-      <c r="N37" s="160"/>
-      <c r="O37" s="160"/>
-      <c r="P37" s="160"/>
-      <c r="Q37" s="160"/>
-      <c r="R37" s="160"/>
-      <c r="S37" s="160"/>
+      <c r="M37" s="168" t="s">
+        <v>79</v>
+      </c>
+      <c r="N37" s="168"/>
+      <c r="O37" s="168"/>
+      <c r="P37" s="168"/>
+      <c r="Q37" s="168"/>
+      <c r="R37" s="168"/>
+      <c r="S37" s="168"/>
     </row>
     <row r="38" spans="2:20" customFormat="1">
       <c r="B38" s="105"/>
       <c r="C38" s="114"/>
-      <c r="M38" s="147" t="s">
-        <v>82</v>
+      <c r="M38" s="138" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="2:20" customFormat="1">
       <c r="B39" s="105"/>
       <c r="C39" s="114"/>
-      <c r="M39" s="161" t="s">
-        <v>83</v>
-      </c>
-      <c r="N39" s="161"/>
-      <c r="O39" s="161"/>
-      <c r="P39" s="161"/>
-      <c r="Q39" s="161"/>
-      <c r="R39" s="161"/>
-      <c r="S39" s="161"/>
+      <c r="M39" s="169" t="s">
+        <v>81</v>
+      </c>
+      <c r="N39" s="169"/>
+      <c r="O39" s="169"/>
+      <c r="P39" s="169"/>
+      <c r="Q39" s="169"/>
+      <c r="R39" s="169"/>
+      <c r="S39" s="169"/>
     </row>
     <row r="40" spans="2:20" customFormat="1">
       <c r="B40" s="105"/>
@@ -4849,7 +4856,7 @@
         <v>35</v>
       </c>
       <c r="G46" s="114" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H46" s="114"/>
       <c r="I46" s="114"/>
@@ -4863,7 +4870,7 @@
         <v>3600</v>
       </c>
       <c r="G47" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="2:20" customFormat="1">
@@ -4873,7 +4880,7 @@
         <v>9.7222222222222224E-3</v>
       </c>
       <c r="G48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:64" customFormat="1">

</xml_diff>